<commit_message>
UPDATE: STE2 structure, 4 Neurotensin complex structures, some new beta and gamma uniprots
</commit_message>
<xml_diff>
--- a/structure_data/Class_D_Annotation.xlsx
+++ b/structure_data/Class_D_Annotation.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ntv489/Dropbox (GloriamGroup)/GPCRDB_Project_Alignments_and_Similarities/Class_D_alignment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ntv489/pvagrant/shared/data/protwis/gpcr/structure_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="SegEnds_Xtal_Prot#" sheetId="1" r:id="rId1"/>
@@ -85,9 +85,6 @@
     <t>_wt</t>
   </si>
   <si>
-    <t>XXXX</t>
-  </si>
-  <si>
     <t>ste2_yeast</t>
   </si>
   <si>
@@ -350,6 +347,9 @@
   </si>
   <si>
     <t>D1e1x</t>
+  </si>
+  <si>
+    <t>7AD3</t>
   </si>
 </sst>
 </file>
@@ -827,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BT3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AD8" sqref="AD8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -903,7 +903,7 @@
   <sheetData>
     <row r="1" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -912,22 +912,22 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" t="s">
         <v>94</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>95</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>96</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>97</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>98</v>
-      </c>
-      <c r="O1" t="s">
-        <v>99</v>
       </c>
       <c r="Q1" t="s">
         <v>2</v>
@@ -936,10 +936,10 @@
         <v>3</v>
       </c>
       <c r="U1" t="s">
+        <v>64</v>
+      </c>
+      <c r="W1" t="s">
         <v>65</v>
-      </c>
-      <c r="W1" t="s">
-        <v>66</v>
       </c>
       <c r="Y1" t="s">
         <v>4</v>
@@ -948,10 +948,10 @@
         <v>5</v>
       </c>
       <c r="AC1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE1" t="s">
         <v>103</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>104</v>
       </c>
       <c r="AG1" t="s">
         <v>6</v>
@@ -960,10 +960,10 @@
         <v>7</v>
       </c>
       <c r="AK1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM1" t="s">
         <v>69</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>70</v>
       </c>
       <c r="AO1" t="s">
         <v>8</v>
@@ -972,10 +972,10 @@
         <v>9</v>
       </c>
       <c r="AS1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU1" t="s">
         <v>72</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>73</v>
       </c>
       <c r="AW1" t="s">
         <v>10</v>
@@ -984,10 +984,10 @@
         <v>11</v>
       </c>
       <c r="BA1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BC1" t="s">
         <v>75</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>76</v>
       </c>
       <c r="BE1" t="s">
         <v>12</v>
@@ -996,10 +996,10 @@
         <v>13</v>
       </c>
       <c r="BI1" t="s">
+        <v>77</v>
+      </c>
+      <c r="BK1" t="s">
         <v>78</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>79</v>
       </c>
       <c r="BM1" t="s">
         <v>14</v>
@@ -1008,13 +1008,13 @@
         <v>15</v>
       </c>
       <c r="BQ1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="BS1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BT1" t="s">
         <v>82</v>
-      </c>
-      <c r="BT1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:72" x14ac:dyDescent="0.2">
@@ -1023,7 +1023,7 @@
         <v>ste2_yeast__wt</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
@@ -1085,10 +1085,10 @@
         <v>72</v>
       </c>
       <c r="U2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="W2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="X2" t="str">
         <f>IFERROR(MID(VLOOKUP($B2,Seqs!$A:$C,3,0),Y2,1),"")</f>
@@ -1133,10 +1133,10 @@
         <v>155</v>
       </c>
       <c r="AK2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AM2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AN2" t="str">
         <f>IFERROR(MID(VLOOKUP($B2,Seqs!$A:$C,3,0),AO2,1),"")</f>
@@ -1153,10 +1153,10 @@
         <v>195</v>
       </c>
       <c r="AS2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AU2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AV2" t="str">
         <f>IFERROR(MID(VLOOKUP($B2,Seqs!$A:$C,3,0),AW2,1),"")</f>
@@ -1173,10 +1173,10 @@
         <v>236</v>
       </c>
       <c r="BA2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BC2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BD2" t="str">
         <f>IFERROR(MID(VLOOKUP($B2,Seqs!$A:$C,3,0),BE2,1),"")</f>
@@ -1193,10 +1193,10 @@
         <v>268</v>
       </c>
       <c r="BI2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BK2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BL2" t="str">
         <f>IFERROR(MID(VLOOKUP($B2,Seqs!$A:$C,3,0),BM2,1),"")</f>
@@ -1217,26 +1217,26 @@
         <v/>
       </c>
       <c r="BQ2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BR2" t="str">
         <f>IFERROR(MID(VLOOKUP($B2,Seqs!$A:$C,3,0),BS2,1),"")</f>
         <v/>
       </c>
       <c r="BS2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>CONCATENATE(B3,"_",C3)</f>
-        <v>ste2_yeast_XXXX</v>
+        <v>ste2_yeast_7AD3</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="D3" t="str">
         <f>IFERROR(MID(VLOOKUP($B3,Seqs!$A:$C,3,0),E3,1),"")</f>
@@ -1295,10 +1295,10 @@
         <v>72</v>
       </c>
       <c r="U3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="W3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="X3" t="str">
         <f>IFERROR(MID(VLOOKUP($B3,Seqs!$A:$C,3,0),Y3,1),"")</f>
@@ -1343,10 +1343,10 @@
         <v>155</v>
       </c>
       <c r="AK3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AM3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AN3" t="str">
         <f>IFERROR(MID(VLOOKUP($B3,Seqs!$A:$C,3,0),AO3,1),"")</f>
@@ -1363,10 +1363,10 @@
         <v>195</v>
       </c>
       <c r="AS3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AU3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AV3" t="str">
         <f>IFERROR(MID(VLOOKUP($B3,Seqs!$A:$C,3,0),AW3,1),"")</f>
@@ -1383,10 +1383,10 @@
         <v>236</v>
       </c>
       <c r="BA3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BC3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BD3" t="str">
         <f>IFERROR(MID(VLOOKUP($B3,Seqs!$A:$C,3,0),BE3,1),"")</f>
@@ -1403,10 +1403,10 @@
         <v>268</v>
       </c>
       <c r="BI3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BK3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BL3" t="str">
         <f>IFERROR(MID(VLOOKUP($B3,Seqs!$A:$C,3,0),BM3,1),"")</f>
@@ -1427,14 +1427,14 @@
         <v/>
       </c>
       <c r="BQ3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BR3" t="str">
         <f>IFERROR(MID(VLOOKUP($B3,Seqs!$A:$C,3,0),BS3,1),"")</f>
         <v/>
       </c>
       <c r="BS3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1471,28 +1471,28 @@
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" t="s">
         <v>94</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>95</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>96</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>97</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>98</v>
-      </c>
-      <c r="H1" t="s">
-        <v>99</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
@@ -1501,10 +1501,10 @@
         <v>3</v>
       </c>
       <c r="K1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" t="s">
         <v>65</v>
-      </c>
-      <c r="L1" t="s">
-        <v>66</v>
       </c>
       <c r="M1" t="s">
         <v>4</v>
@@ -1513,10 +1513,10 @@
         <v>5</v>
       </c>
       <c r="O1" t="s">
+        <v>102</v>
+      </c>
+      <c r="P1" t="s">
         <v>103</v>
-      </c>
-      <c r="P1" t="s">
-        <v>104</v>
       </c>
       <c r="Q1" t="s">
         <v>6</v>
@@ -1525,10 +1525,10 @@
         <v>7</v>
       </c>
       <c r="S1" t="s">
+        <v>68</v>
+      </c>
+      <c r="T1" t="s">
         <v>69</v>
-      </c>
-      <c r="T1" t="s">
-        <v>70</v>
       </c>
       <c r="U1" t="s">
         <v>8</v>
@@ -1537,10 +1537,10 @@
         <v>9</v>
       </c>
       <c r="W1" t="s">
+        <v>71</v>
+      </c>
+      <c r="X1" t="s">
         <v>72</v>
-      </c>
-      <c r="X1" t="s">
-        <v>73</v>
       </c>
       <c r="Y1" t="s">
         <v>10</v>
@@ -1549,10 +1549,10 @@
         <v>11</v>
       </c>
       <c r="AA1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB1" t="s">
         <v>75</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>76</v>
       </c>
       <c r="AC1" t="s">
         <v>12</v>
@@ -1561,10 +1561,10 @@
         <v>13</v>
       </c>
       <c r="AE1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF1" t="s">
         <v>78</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>79</v>
       </c>
       <c r="AG1" t="s">
         <v>14</v>
@@ -1579,7 +1579,7 @@
         <v>ste2_yeast__wt</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <f>IFERROR(50+VLOOKUP($A2,'SegEnds_Xtal_Prot#'!$A:$CN,5,FALSE)-VLOOKUP($B2,'SegEnds_NonXtal_Prot#'!$B:$BX,4,FALSE),"-")</f>
@@ -1614,10 +1614,10 @@
         <v>60</v>
       </c>
       <c r="K2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M2">
         <f>IFERROR(50+VLOOKUP($A2,'SegEnds_Xtal_Prot#'!$A:$CN,25,FALSE)-VLOOKUP($B2,'SegEnds_NonXtal_Prot#'!$B:$BX,19,FALSE),"-")</f>
@@ -1644,10 +1644,10 @@
         <v>56</v>
       </c>
       <c r="S2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U2">
         <f>IFERROR(50+VLOOKUP($A2,'SegEnds_Xtal_Prot#'!$A:$CN,41,FALSE)-VLOOKUP($B2,'SegEnds_NonXtal_Prot#'!$B:$BX,31,FALSE),"-")</f>
@@ -1658,10 +1658,10 @@
         <v>67</v>
       </c>
       <c r="W2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="X2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Y2">
         <f>IFERROR(50+VLOOKUP($A2,'SegEnds_Xtal_Prot#'!$A:$CN,49,FALSE)-VLOOKUP($B2,'SegEnds_NonXtal_Prot#'!$B:$BX,37,FALSE),"-")</f>
@@ -1672,10 +1672,10 @@
         <v>75</v>
       </c>
       <c r="AA2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AB2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AC2">
         <f>IFERROR(50+VLOOKUP($A2,'SegEnds_Xtal_Prot#'!$A:$CN,57,FALSE)-VLOOKUP($B2,'SegEnds_NonXtal_Prot#'!$B:$BX,43,FALSE),"-")</f>
@@ -1686,10 +1686,10 @@
         <v>54</v>
       </c>
       <c r="AE2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AF2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AG2">
         <f>IFERROR(50+VLOOKUP($A2,'SegEnds_Xtal_Prot#'!$A:$CN,65,FALSE)-VLOOKUP($B2,'SegEnds_NonXtal_Prot#'!$B:$BX,49,FALSE),"-")</f>
@@ -1738,25 +1738,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" t="s">
         <v>94</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>95</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>96</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>97</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>98</v>
-      </c>
-      <c r="H1" t="s">
-        <v>99</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
@@ -1765,10 +1765,10 @@
         <v>3</v>
       </c>
       <c r="K1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" t="s">
         <v>65</v>
-      </c>
-      <c r="L1" t="s">
-        <v>66</v>
       </c>
       <c r="M1" t="s">
         <v>4</v>
@@ -1777,10 +1777,10 @@
         <v>5</v>
       </c>
       <c r="O1" t="s">
+        <v>102</v>
+      </c>
+      <c r="P1" t="s">
         <v>103</v>
-      </c>
-      <c r="P1" t="s">
-        <v>104</v>
       </c>
       <c r="Q1" t="s">
         <v>6</v>
@@ -1789,10 +1789,10 @@
         <v>7</v>
       </c>
       <c r="S1" t="s">
+        <v>68</v>
+      </c>
+      <c r="T1" t="s">
         <v>69</v>
-      </c>
-      <c r="T1" t="s">
-        <v>70</v>
       </c>
       <c r="U1" t="s">
         <v>8</v>
@@ -1801,10 +1801,10 @@
         <v>9</v>
       </c>
       <c r="W1" t="s">
+        <v>71</v>
+      </c>
+      <c r="X1" t="s">
         <v>72</v>
-      </c>
-      <c r="X1" t="s">
-        <v>73</v>
       </c>
       <c r="Y1" t="s">
         <v>10</v>
@@ -1813,10 +1813,10 @@
         <v>11</v>
       </c>
       <c r="AA1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB1" t="s">
         <v>75</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>76</v>
       </c>
       <c r="AC1" t="s">
         <v>12</v>
@@ -1825,10 +1825,10 @@
         <v>13</v>
       </c>
       <c r="AE1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF1" t="s">
         <v>78</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>79</v>
       </c>
       <c r="AG1" t="s">
         <v>14</v>
@@ -1839,7 +1839,7 @@
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="str">
         <f>VLOOKUP(A2,Seqs!$A:$D,2,FALSE)</f>
@@ -1878,10 +1878,10 @@
         <v>60</v>
       </c>
       <c r="K2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M2">
         <f>VLOOKUP($B2&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,13,FALSE)</f>
@@ -1908,10 +1908,10 @@
         <v>56</v>
       </c>
       <c r="S2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U2">
         <f>VLOOKUP($B2&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,21,FALSE)</f>
@@ -1922,10 +1922,10 @@
         <v>67</v>
       </c>
       <c r="W2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="X2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Y2">
         <f>VLOOKUP($B2&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,25,FALSE)</f>
@@ -1936,10 +1936,10 @@
         <v>75</v>
       </c>
       <c r="AA2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AB2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AC2">
         <f>VLOOKUP($B2&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,29,FALSE)</f>
@@ -1950,10 +1950,10 @@
         <v>54</v>
       </c>
       <c r="AE2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AF2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AG2">
         <f>VLOOKUP($B2&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,33,FALSE)</f>
@@ -1966,7 +1966,7 @@
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" t="str">
         <f>VLOOKUP(A3,Seqs!$A:$D,2,FALSE)</f>
@@ -2005,10 +2005,10 @@
         <v>60</v>
       </c>
       <c r="K3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M3">
         <f>VLOOKUP($B3&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,13,FALSE)</f>
@@ -2035,10 +2035,10 @@
         <v>56</v>
       </c>
       <c r="S3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U3">
         <f>VLOOKUP($B3&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,21,FALSE)</f>
@@ -2049,10 +2049,10 @@
         <v>67</v>
       </c>
       <c r="W3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="X3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Y3">
         <f>VLOOKUP($B3&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,25,FALSE)</f>
@@ -2063,10 +2063,10 @@
         <v>75</v>
       </c>
       <c r="AA3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AB3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AC3">
         <f>VLOOKUP($B3&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,29,FALSE)</f>
@@ -2077,10 +2077,10 @@
         <v>54</v>
       </c>
       <c r="AE3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AF3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AG3">
         <f>VLOOKUP($B3&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,33,FALSE)</f>
@@ -2093,7 +2093,7 @@
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" t="str">
         <f>VLOOKUP(A4,Seqs!$A:$D,2,FALSE)</f>
@@ -2132,10 +2132,10 @@
         <v>60</v>
       </c>
       <c r="K4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M4">
         <f>VLOOKUP($B4&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,13,FALSE)</f>
@@ -2162,10 +2162,10 @@
         <v>56</v>
       </c>
       <c r="S4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U4">
         <f>VLOOKUP($B4&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,21,FALSE)</f>
@@ -2176,10 +2176,10 @@
         <v>67</v>
       </c>
       <c r="W4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="X4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Y4">
         <f>VLOOKUP($B4&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,25,FALSE)</f>
@@ -2190,10 +2190,10 @@
         <v>75</v>
       </c>
       <c r="AA4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AB4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AC4">
         <f>VLOOKUP($B4&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,29,FALSE)</f>
@@ -2204,10 +2204,10 @@
         <v>54</v>
       </c>
       <c r="AE4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AF4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AG4">
         <f>VLOOKUP($B4&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,33,FALSE)</f>
@@ -2220,7 +2220,7 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" t="str">
         <f>VLOOKUP(A5,Seqs!$A:$D,2,FALSE)</f>
@@ -2259,10 +2259,10 @@
         <v>60</v>
       </c>
       <c r="K5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M5">
         <f>VLOOKUP($B5&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,13,FALSE)</f>
@@ -2289,10 +2289,10 @@
         <v>56</v>
       </c>
       <c r="S5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U5">
         <f>VLOOKUP($B5&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,21,FALSE)</f>
@@ -2303,10 +2303,10 @@
         <v>67</v>
       </c>
       <c r="W5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="X5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Y5">
         <f>VLOOKUP($B5&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,25,FALSE)</f>
@@ -2317,10 +2317,10 @@
         <v>75</v>
       </c>
       <c r="AA5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AB5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AC5">
         <f>VLOOKUP($B5&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,29,FALSE)</f>
@@ -2331,10 +2331,10 @@
         <v>54</v>
       </c>
       <c r="AE5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AF5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AG5">
         <f>VLOOKUP($B5&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,33,FALSE)</f>
@@ -2347,7 +2347,7 @@
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" t="str">
         <f>VLOOKUP(A6,Seqs!$A:$D,2,FALSE)</f>
@@ -2386,10 +2386,10 @@
         <v>60</v>
       </c>
       <c r="K6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M6">
         <f>VLOOKUP($B6&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,13,FALSE)</f>
@@ -2416,10 +2416,10 @@
         <v>56</v>
       </c>
       <c r="S6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U6">
         <f>VLOOKUP($B6&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,21,FALSE)</f>
@@ -2430,10 +2430,10 @@
         <v>67</v>
       </c>
       <c r="W6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="X6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Y6">
         <f>VLOOKUP($B6&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,25,FALSE)</f>
@@ -2444,10 +2444,10 @@
         <v>75</v>
       </c>
       <c r="AA6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AB6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AC6">
         <f>VLOOKUP($B6&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,29,FALSE)</f>
@@ -2458,10 +2458,10 @@
         <v>54</v>
       </c>
       <c r="AE6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AF6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AG6">
         <f>VLOOKUP($B6&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,33,FALSE)</f>
@@ -2474,7 +2474,7 @@
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" t="str">
         <f>VLOOKUP(A7,Seqs!$A:$D,2,FALSE)</f>
@@ -2513,10 +2513,10 @@
         <v>60</v>
       </c>
       <c r="K7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M7">
         <f>VLOOKUP($B7&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,13,FALSE)</f>
@@ -2543,10 +2543,10 @@
         <v>56</v>
       </c>
       <c r="S7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U7">
         <f>VLOOKUP($B7&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,21,FALSE)</f>
@@ -2557,10 +2557,10 @@
         <v>67</v>
       </c>
       <c r="W7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="X7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Y7">
         <f>VLOOKUP($B7&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,25,FALSE)</f>
@@ -2571,10 +2571,10 @@
         <v>75</v>
       </c>
       <c r="AA7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AB7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AC7">
         <f>VLOOKUP($B7&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,29,FALSE)</f>
@@ -2585,10 +2585,10 @@
         <v>54</v>
       </c>
       <c r="AE7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AF7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AG7">
         <f>VLOOKUP($B7&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,33,FALSE)</f>
@@ -2601,7 +2601,7 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" t="str">
         <f>VLOOKUP(A8,Seqs!$A:$D,2,FALSE)</f>
@@ -2640,10 +2640,10 @@
         <v>60</v>
       </c>
       <c r="K8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M8">
         <f>VLOOKUP($B8&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,13,FALSE)</f>
@@ -2670,10 +2670,10 @@
         <v>56</v>
       </c>
       <c r="S8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U8">
         <f>VLOOKUP($B8&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,21,FALSE)</f>
@@ -2684,10 +2684,10 @@
         <v>67</v>
       </c>
       <c r="W8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="X8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Y8">
         <f>VLOOKUP($B8&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,25,FALSE)</f>
@@ -2698,10 +2698,10 @@
         <v>75</v>
       </c>
       <c r="AA8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AB8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AC8">
         <f>VLOOKUP($B8&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,29,FALSE)</f>
@@ -2712,10 +2712,10 @@
         <v>54</v>
       </c>
       <c r="AE8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AF8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AG8">
         <f>VLOOKUP($B8&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,33,FALSE)</f>
@@ -2728,7 +2728,7 @@
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" t="str">
         <f>VLOOKUP(A9,Seqs!$A:$D,2,FALSE)</f>
@@ -2767,10 +2767,10 @@
         <v>60</v>
       </c>
       <c r="K9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M9">
         <f>VLOOKUP($B9&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,13,FALSE)</f>
@@ -2797,10 +2797,10 @@
         <v>56</v>
       </c>
       <c r="S9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U9">
         <f>VLOOKUP($B9&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,21,FALSE)</f>
@@ -2811,10 +2811,10 @@
         <v>67</v>
       </c>
       <c r="W9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="X9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Y9">
         <f>VLOOKUP($B9&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,25,FALSE)</f>
@@ -2825,10 +2825,10 @@
         <v>75</v>
       </c>
       <c r="AA9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AB9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AC9">
         <f>VLOOKUP($B9&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,29,FALSE)</f>
@@ -2839,10 +2839,10 @@
         <v>54</v>
       </c>
       <c r="AE9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AF9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AG9">
         <f>VLOOKUP($B9&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,33,FALSE)</f>
@@ -2855,7 +2855,7 @@
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B10" t="str">
         <f>VLOOKUP(A10,Seqs!$A:$D,2,FALSE)</f>
@@ -2894,10 +2894,10 @@
         <v>60</v>
       </c>
       <c r="K10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M10">
         <f>VLOOKUP($B10&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,13,FALSE)</f>
@@ -2924,10 +2924,10 @@
         <v>56</v>
       </c>
       <c r="S10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U10">
         <f>VLOOKUP($B10&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,21,FALSE)</f>
@@ -2938,10 +2938,10 @@
         <v>67</v>
       </c>
       <c r="W10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="X10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Y10">
         <f>VLOOKUP($B10&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,25,FALSE)</f>
@@ -2952,10 +2952,10 @@
         <v>75</v>
       </c>
       <c r="AA10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AB10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AC10">
         <f>VLOOKUP($B10&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,29,FALSE)</f>
@@ -2966,10 +2966,10 @@
         <v>54</v>
       </c>
       <c r="AE10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AF10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AG10">
         <f>VLOOKUP($B10&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,33,FALSE)</f>
@@ -2982,7 +2982,7 @@
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B11" t="str">
         <f>VLOOKUP(A11,Seqs!$A:$D,2,FALSE)</f>
@@ -3020,10 +3020,10 @@
         <v>60</v>
       </c>
       <c r="K11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M11">
         <f>VLOOKUP($B11&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,13,FALSE)</f>
@@ -3050,10 +3050,10 @@
         <v>56</v>
       </c>
       <c r="S11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U11">
         <f>VLOOKUP($B11&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,21,FALSE)</f>
@@ -3064,10 +3064,10 @@
         <v>67</v>
       </c>
       <c r="W11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="X11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Y11">
         <f>VLOOKUP($B11&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,25,FALSE)</f>
@@ -3078,10 +3078,10 @@
         <v>75</v>
       </c>
       <c r="AA11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AB11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AC11">
         <f>VLOOKUP($B11&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,29,FALSE)</f>
@@ -3092,10 +3092,10 @@
         <v>54</v>
       </c>
       <c r="AE11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AF11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AG11">
         <f>VLOOKUP($B11&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,33,FALSE)</f>
@@ -3108,7 +3108,7 @@
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B12" t="str">
         <f>VLOOKUP(A12,Seqs!$A:$D,2,FALSE)</f>
@@ -3147,10 +3147,10 @@
         <v>60</v>
       </c>
       <c r="K12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M12">
         <f>VLOOKUP($B12&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,13,FALSE)</f>
@@ -3177,10 +3177,10 @@
         <v>56</v>
       </c>
       <c r="S12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U12">
         <f>VLOOKUP($B12&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,21,FALSE)</f>
@@ -3191,10 +3191,10 @@
         <v>67</v>
       </c>
       <c r="W12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="X12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Y12">
         <f>VLOOKUP($B12&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,25,FALSE)</f>
@@ -3205,10 +3205,10 @@
         <v>75</v>
       </c>
       <c r="AA12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AB12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AC12">
         <f>VLOOKUP($B12&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,29,FALSE)</f>
@@ -3219,10 +3219,10 @@
         <v>54</v>
       </c>
       <c r="AE12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AF12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AG12">
         <f>VLOOKUP($B12&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,33,FALSE)</f>
@@ -3235,7 +3235,7 @@
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B13" t="str">
         <f>VLOOKUP(A13,Seqs!$A:$D,2,FALSE)</f>
@@ -3274,10 +3274,10 @@
         <v>60</v>
       </c>
       <c r="K13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M13">
         <f>VLOOKUP($B13&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,13,FALSE)</f>
@@ -3304,10 +3304,10 @@
         <v>56</v>
       </c>
       <c r="S13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U13">
         <f>VLOOKUP($B13&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,21,FALSE)</f>
@@ -3318,10 +3318,10 @@
         <v>67</v>
       </c>
       <c r="W13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="X13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Y13">
         <f>VLOOKUP($B13&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,25,FALSE)</f>
@@ -3332,10 +3332,10 @@
         <v>75</v>
       </c>
       <c r="AA13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AB13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AC13">
         <f>VLOOKUP($B13&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,29,FALSE)</f>
@@ -3346,10 +3346,10 @@
         <v>54</v>
       </c>
       <c r="AE13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AF13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AG13">
         <f>VLOOKUP($B13&amp;"__wt",'SegEnds_Xtal_BW#'!$A:$AR,33,FALSE)</f>
@@ -3369,7 +3369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BX13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
@@ -3435,184 +3435,184 @@
   <sheetData>
     <row r="1" spans="1:76" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="G1" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="J1" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="P1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="S1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="V1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="X1" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>104</v>
       </c>
       <c r="Y1" s="5" t="s">
         <v>6</v>
       </c>
       <c r="Z1" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AA1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="AB1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC1" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD1" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="AC1" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD1" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="AE1" s="5" t="s">
         <v>8</v>
       </c>
       <c r="AF1" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AG1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="AH1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ1" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="AI1" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="AJ1" s="5" t="s">
-        <v>73</v>
       </c>
       <c r="AK1" s="5" t="s">
         <v>10</v>
       </c>
       <c r="AL1" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AM1" s="5" t="s">
         <v>11</v>
       </c>
       <c r="AN1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AO1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="AP1" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="AO1" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="AP1" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="AQ1" s="5" t="s">
         <v>12</v>
       </c>
       <c r="AR1" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AS1" s="5" t="s">
         <v>13</v>
       </c>
       <c r="AT1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AU1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="AV1" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="AU1" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="AV1" s="5" t="s">
-        <v>79</v>
       </c>
       <c r="AW1" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AX1" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AY1" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AZ1" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="BA1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="BA1" s="6" t="s">
+      <c r="BB1" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="BB1" s="5" t="s">
-        <v>82</v>
-      </c>
       <c r="BE1" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="BF1" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="BF1" s="5" t="s">
+      <c r="BG1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="BG1" s="5" t="s">
+      <c r="BH1" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="BH1" s="5" t="s">
+      <c r="BI1" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="BI1" s="5" t="s">
+      <c r="BJ1" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="BJ1" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="BK1" s="5" t="s">
         <v>2</v>
@@ -3663,7 +3663,7 @@
         <v>ste2_yeast__wt</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" t="str">
         <f>VLOOKUP(B2,Seqs!A:B,2,FALSE)</f>
@@ -3714,13 +3714,13 @@
         <v>72</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S2">
         <f>VLOOKUP($B2,'SegEnds_NonXtal_BW#'!$A:$AR,13,FALSE)+T2-50</f>
@@ -3756,13 +3756,13 @@
         <v>155</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AE2" s="1">
         <f>VLOOKUP($B2,'SegEnds_NonXtal_BW#'!$A:$AR,21,FALSE)+AF2-50</f>
@@ -3776,13 +3776,13 @@
         <v>195</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AJ2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AK2">
         <f>VLOOKUP($B2,'SegEnds_NonXtal_BW#'!$A:$AR,25,FALSE)+AL2-50</f>
@@ -3796,13 +3796,13 @@
         <v>236</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AO2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AP2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AQ2">
         <f>VLOOKUP($B2,'SegEnds_NonXtal_BW#'!$A:$AR,29,FALSE)+AR2-50</f>
@@ -3816,13 +3816,13 @@
         <v>268</v>
       </c>
       <c r="AT2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AU2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AV2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AW2">
         <f>VLOOKUP($B2,'SegEnds_NonXtal_BW#'!$A:$AR,33,FALSE)+AX2-50</f>
@@ -3836,13 +3836,13 @@
         <v>306</v>
       </c>
       <c r="AZ2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BA2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BB2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BD2" t="b">
         <f>IF(COUNTIF('SegEnds_Xtal_Prot#'!B:B,'SegEnds_NonXtal_Prot#'!B2)&gt;0,IF(COUNTIF(BK2:BX2,TRUE)=14,TRUE,FALSE),"NoXtal")</f>
@@ -3935,7 +3935,7 @@
         <v>A0A0W0DD93_CANGB__wt</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" t="str">
         <f>VLOOKUP(B3,Seqs!A:B,2,FALSE)</f>
@@ -3986,13 +3986,13 @@
         <v>65</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S3">
         <f>VLOOKUP($B3,'SegEnds_NonXtal_BW#'!$A:$AR,13,FALSE)+T3-50</f>
@@ -4028,13 +4028,13 @@
         <v>148</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AE3" s="1">
         <f>VLOOKUP($B3,'SegEnds_NonXtal_BW#'!$A:$AR,21,FALSE)+AF3-50</f>
@@ -4048,13 +4048,13 @@
         <v>188</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AI3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AJ3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AK3">
         <f>VLOOKUP($B3,'SegEnds_NonXtal_BW#'!$A:$AR,25,FALSE)+AL3-50</f>
@@ -4068,13 +4068,13 @@
         <v>229</v>
       </c>
       <c r="AN3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AO3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AP3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AQ3">
         <f>VLOOKUP($B3,'SegEnds_NonXtal_BW#'!$A:$AR,29,FALSE)+AR3-50</f>
@@ -4088,13 +4088,13 @@
         <v>261</v>
       </c>
       <c r="AT3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AU3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AV3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AW3">
         <f>VLOOKUP($B3,'SegEnds_NonXtal_BW#'!$A:$AR,33,FALSE)+AX3-50</f>
@@ -4108,13 +4108,13 @@
         <v>299</v>
       </c>
       <c r="AZ3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BA3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BB3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BD3" t="str">
         <f>IF(COUNTIF('SegEnds_Xtal_Prot#'!B:B,'SegEnds_NonXtal_Prot#'!B3)&gt;0,IF(COUNTIF(BK3:BX3,TRUE)=14,TRUE,FALSE),"NoXtal")</f>
@@ -4207,7 +4207,7 @@
         <v>Q8WZM9_SORMA__wt</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" t="str">
         <f>VLOOKUP(B4,Seqs!A:B,2,FALSE)</f>
@@ -4258,13 +4258,13 @@
         <v>89</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S4">
         <f>VLOOKUP($B4,'SegEnds_NonXtal_BW#'!$A:$AR,13,FALSE)+T4-50</f>
@@ -4300,13 +4300,13 @@
         <v>174</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AE4" s="1">
         <f>VLOOKUP($B4,'SegEnds_NonXtal_BW#'!$A:$AR,21,FALSE)+AF4-50</f>
@@ -4320,13 +4320,13 @@
         <v>213</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AI4" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AJ4" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AK4">
         <f>VLOOKUP($B4,'SegEnds_NonXtal_BW#'!$A:$AR,25,FALSE)+AL4-50</f>
@@ -4340,13 +4340,13 @@
         <v>254</v>
       </c>
       <c r="AN4" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AO4" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AP4" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AQ4">
         <f>VLOOKUP($B4,'SegEnds_NonXtal_BW#'!$A:$AR,29,FALSE)+AR4-50</f>
@@ -4360,13 +4360,13 @@
         <v>288</v>
       </c>
       <c r="AT4" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AU4" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AV4" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AW4">
         <f>VLOOKUP($B4,'SegEnds_NonXtal_BW#'!$A:$AR,33,FALSE)+AX4-50</f>
@@ -4380,13 +4380,13 @@
         <v>324</v>
       </c>
       <c r="AZ4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BA4" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BB4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BD4" t="str">
         <f>IF(COUNTIF('SegEnds_Xtal_Prot#'!B:B,'SegEnds_NonXtal_Prot#'!B4)&gt;0,IF(COUNTIF(BK4:BX4,TRUE)=14,TRUE,FALSE),"NoXtal")</f>
@@ -4479,7 +4479,7 @@
         <v>B1GVB8_PENCH__wt</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" t="str">
         <f>VLOOKUP(B5,Seqs!A:B,2,FALSE)</f>
@@ -4530,13 +4530,13 @@
         <v>65</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S5">
         <f>VLOOKUP($B5,'SegEnds_NonXtal_BW#'!$A:$AR,13,FALSE)+T5-50</f>
@@ -4572,13 +4572,13 @@
         <v>150</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AC5" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AE5" s="1">
         <f>VLOOKUP($B5,'SegEnds_NonXtal_BW#'!$A:$AR,21,FALSE)+AF5-50</f>
@@ -4592,13 +4592,13 @@
         <v>189</v>
       </c>
       <c r="AH5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AI5" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AJ5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AK5">
         <f>VLOOKUP($B5,'SegEnds_NonXtal_BW#'!$A:$AR,25,FALSE)+AL5-50</f>
@@ -4612,13 +4612,13 @@
         <v>231</v>
       </c>
       <c r="AN5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AO5" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AP5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AQ5">
         <f>VLOOKUP($B5,'SegEnds_NonXtal_BW#'!$A:$AR,29,FALSE)+AR5-50</f>
@@ -4632,13 +4632,13 @@
         <v>263</v>
       </c>
       <c r="AT5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AU5" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AV5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AW5">
         <f>VLOOKUP($B5,'SegEnds_NonXtal_BW#'!$A:$AR,33,FALSE)+AX5-50</f>
@@ -4652,13 +4652,13 @@
         <v>297</v>
       </c>
       <c r="AZ5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BA5" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BB5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BD5" t="str">
         <f>IF(COUNTIF('SegEnds_Xtal_Prot#'!B:B,'SegEnds_NonXtal_Prot#'!B5)&gt;0,IF(COUNTIF(BK5:BX5,TRUE)=14,TRUE,FALSE),"NoXtal")</f>
@@ -4751,7 +4751,7 @@
         <v>mam2_schpo__wt</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" t="str">
         <f>VLOOKUP(B6,Seqs!A:B,2,FALSE)</f>
@@ -4802,13 +4802,13 @@
         <v>71</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S6">
         <f>VLOOKUP($B6,'SegEnds_NonXtal_BW#'!$A:$AR,13,FALSE)+T6-50</f>
@@ -4844,13 +4844,13 @@
         <v>154</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AC6" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AE6" s="1">
         <f>VLOOKUP($B6,'SegEnds_NonXtal_BW#'!$A:$AR,21,FALSE)+AF6-50</f>
@@ -4864,13 +4864,13 @@
         <v>192</v>
       </c>
       <c r="AH6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AI6" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AJ6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AK6">
         <f>VLOOKUP($B6,'SegEnds_NonXtal_BW#'!$A:$AR,25,FALSE)+AL6-50</f>
@@ -4884,13 +4884,13 @@
         <v>239</v>
       </c>
       <c r="AN6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AO6" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AP6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AQ6">
         <f>VLOOKUP($B6,'SegEnds_NonXtal_BW#'!$A:$AR,29,FALSE)+AR6-50</f>
@@ -4904,13 +4904,13 @@
         <v>271</v>
       </c>
       <c r="AT6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AU6" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AV6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AW6">
         <f>VLOOKUP($B6,'SegEnds_NonXtal_BW#'!$A:$AR,33,FALSE)+AX6-50</f>
@@ -4924,13 +4924,13 @@
         <v>306</v>
       </c>
       <c r="AZ6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BA6" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BB6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BD6" t="str">
         <f>IF(COUNTIF('SegEnds_Xtal_Prot#'!B:B,'SegEnds_NonXtal_Prot#'!B6)&gt;0,IF(COUNTIF(BK6:BX6,TRUE)=14,TRUE,FALSE),"NoXtal")</f>
@@ -5023,7 +5023,7 @@
         <v>Q4WYU8_ASPFU__wt</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" t="str">
         <f>VLOOKUP(B7,Seqs!A:B,2,FALSE)</f>
@@ -5074,13 +5074,13 @@
         <v>60</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S7">
         <f>VLOOKUP($B7,'SegEnds_NonXtal_BW#'!$A:$AR,13,FALSE)+T7-50</f>
@@ -5116,13 +5116,13 @@
         <v>145</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AC7" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AE7" s="1">
         <f>VLOOKUP($B7,'SegEnds_NonXtal_BW#'!$A:$AR,21,FALSE)+AF7-50</f>
@@ -5136,13 +5136,13 @@
         <v>184</v>
       </c>
       <c r="AH7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AI7" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AJ7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AK7">
         <f>VLOOKUP($B7,'SegEnds_NonXtal_BW#'!$A:$AR,25,FALSE)+AL7-50</f>
@@ -5156,13 +5156,13 @@
         <v>226</v>
       </c>
       <c r="AN7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AO7" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AP7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AQ7">
         <f>VLOOKUP($B7,'SegEnds_NonXtal_BW#'!$A:$AR,29,FALSE)+AR7-50</f>
@@ -5176,13 +5176,13 @@
         <v>258</v>
       </c>
       <c r="AT7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AU7" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AV7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AW7">
         <f>VLOOKUP($B7,'SegEnds_NonXtal_BW#'!$A:$AR,33,FALSE)+AX7-50</f>
@@ -5196,13 +5196,13 @@
         <v>292</v>
       </c>
       <c r="AZ7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BA7" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BB7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BD7" t="str">
         <f>IF(COUNTIF('SegEnds_Xtal_Prot#'!B:B,'SegEnds_NonXtal_Prot#'!B7)&gt;0,IF(COUNTIF(BK7:BX7,TRUE)=14,TRUE,FALSE),"NoXtal")</f>
@@ -5295,7 +5295,7 @@
         <v>Q8NIR1_NEUCS__wt</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" t="str">
         <f>VLOOKUP(B8,Seqs!A:B,2,FALSE)</f>
@@ -5346,13 +5346,13 @@
         <v>91</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S8">
         <f>VLOOKUP($B8,'SegEnds_NonXtal_BW#'!$A:$AR,13,FALSE)+T8-50</f>
@@ -5388,13 +5388,13 @@
         <v>176</v>
       </c>
       <c r="AB8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AC8" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AE8" s="1">
         <f>VLOOKUP($B8,'SegEnds_NonXtal_BW#'!$A:$AR,21,FALSE)+AF8-50</f>
@@ -5408,13 +5408,13 @@
         <v>215</v>
       </c>
       <c r="AH8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AI8" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AJ8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AK8">
         <f>VLOOKUP($B8,'SegEnds_NonXtal_BW#'!$A:$AR,25,FALSE)+AL8-50</f>
@@ -5428,13 +5428,13 @@
         <v>256</v>
       </c>
       <c r="AN8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AO8" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AP8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AQ8">
         <f>VLOOKUP($B8,'SegEnds_NonXtal_BW#'!$A:$AR,29,FALSE)+AR8-50</f>
@@ -5448,13 +5448,13 @@
         <v>290</v>
       </c>
       <c r="AT8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AU8" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AV8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AW8">
         <f>VLOOKUP($B8,'SegEnds_NonXtal_BW#'!$A:$AR,33,FALSE)+AX8-50</f>
@@ -5468,13 +5468,13 @@
         <v>326</v>
       </c>
       <c r="AZ8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BA8" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BB8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BD8" t="str">
         <f>IF(COUNTIF('SegEnds_Xtal_Prot#'!B:B,'SegEnds_NonXtal_Prot#'!B8)&gt;0,IF(COUNTIF(BK8:BX8,TRUE)=14,TRUE,FALSE),"NoXtal")</f>
@@ -5567,7 +5567,7 @@
         <v>STE2_LACKL__wt</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C9" t="str">
         <f>VLOOKUP(B9,Seqs!A:B,2,FALSE)</f>
@@ -5618,13 +5618,13 @@
         <v>71</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S9">
         <f>VLOOKUP($B9,'SegEnds_NonXtal_BW#'!$A:$AR,13,FALSE)+T9-50</f>
@@ -5660,13 +5660,13 @@
         <v>154</v>
       </c>
       <c r="AB9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AC9" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AE9" s="1">
         <f>VLOOKUP($B9,'SegEnds_NonXtal_BW#'!$A:$AR,21,FALSE)+AF9-50</f>
@@ -5680,13 +5680,13 @@
         <v>194</v>
       </c>
       <c r="AH9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AI9" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AJ9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AK9">
         <f>VLOOKUP($B9,'SegEnds_NonXtal_BW#'!$A:$AR,25,FALSE)+AL9-50</f>
@@ -5700,13 +5700,13 @@
         <v>236</v>
       </c>
       <c r="AN9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AO9" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AP9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AQ9">
         <f>VLOOKUP($B9,'SegEnds_NonXtal_BW#'!$A:$AR,29,FALSE)+AR9-50</f>
@@ -5720,13 +5720,13 @@
         <v>268</v>
       </c>
       <c r="AT9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AU9" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AV9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AW9">
         <f>VLOOKUP($B9,'SegEnds_NonXtal_BW#'!$A:$AR,33,FALSE)+AX9-50</f>
@@ -5740,13 +5740,13 @@
         <v>306</v>
       </c>
       <c r="AZ9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BA9" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BB9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BD9" t="str">
         <f>IF(COUNTIF('SegEnds_Xtal_Prot#'!B:B,'SegEnds_NonXtal_Prot#'!B9)&gt;0,IF(COUNTIF(BK9:BX9,TRUE)=14,TRUE,FALSE),"NoXtal")</f>
@@ -5839,7 +5839,7 @@
         <v>Q6FLY8_CANGA__wt</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C10" t="str">
         <f>VLOOKUP(B10,Seqs!A:B,2,FALSE)</f>
@@ -5890,13 +5890,13 @@
         <v>65</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S10">
         <f>VLOOKUP($B10,'SegEnds_NonXtal_BW#'!$A:$AR,13,FALSE)+T10-50</f>
@@ -5932,13 +5932,13 @@
         <v>148</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AC10" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AE10" s="1">
         <f>VLOOKUP($B10,'SegEnds_NonXtal_BW#'!$A:$AR,21,FALSE)+AF10-50</f>
@@ -5952,13 +5952,13 @@
         <v>188</v>
       </c>
       <c r="AH10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AI10" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AJ10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AK10">
         <f>VLOOKUP($B10,'SegEnds_NonXtal_BW#'!$A:$AR,25,FALSE)+AL10-50</f>
@@ -5972,13 +5972,13 @@
         <v>229</v>
       </c>
       <c r="AN10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AO10" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AP10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AQ10">
         <f>VLOOKUP($B10,'SegEnds_NonXtal_BW#'!$A:$AR,29,FALSE)+AR10-50</f>
@@ -5992,13 +5992,13 @@
         <v>261</v>
       </c>
       <c r="AT10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AU10" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AV10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AW10">
         <f>VLOOKUP($B10,'SegEnds_NonXtal_BW#'!$A:$AR,33,FALSE)+AX10-50</f>
@@ -6012,13 +6012,13 @@
         <v>299</v>
       </c>
       <c r="AZ10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BA10" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BB10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BD10" t="str">
         <f>IF(COUNTIF('SegEnds_Xtal_Prot#'!B:B,'SegEnds_NonXtal_Prot#'!B10)&gt;0,IF(COUNTIF(BK10:BX10,TRUE)=14,TRUE,FALSE),"NoXtal")</f>
@@ -6111,7 +6111,7 @@
         <v>G2YE05_BOTF4__wt</v>
       </c>
       <c r="B11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C11" t="str">
         <f>VLOOKUP(B11,Seqs!A:B,2,FALSE)</f>
@@ -6162,13 +6162,13 @@
         <v>64</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S11">
         <f>VLOOKUP($B11,'SegEnds_NonXtal_BW#'!$A:$AR,13,FALSE)+T11-50</f>
@@ -6204,13 +6204,13 @@
         <v>149</v>
       </c>
       <c r="AB11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AC11" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AE11" s="1">
         <f>VLOOKUP($B11,'SegEnds_NonXtal_BW#'!$A:$AR,21,FALSE)+AF11-50</f>
@@ -6224,13 +6224,13 @@
         <v>188</v>
       </c>
       <c r="AH11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AI11" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AJ11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AK11">
         <f>VLOOKUP($B11,'SegEnds_NonXtal_BW#'!$A:$AR,25,FALSE)+AL11-50</f>
@@ -6244,13 +6244,13 @@
         <v>231</v>
       </c>
       <c r="AN11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AO11" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AP11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AQ11">
         <f>VLOOKUP($B11,'SegEnds_NonXtal_BW#'!$A:$AR,29,FALSE)+AR11-50</f>
@@ -6264,13 +6264,13 @@
         <v>263</v>
       </c>
       <c r="AT11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AU11" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AV11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AW11">
         <f>VLOOKUP($B11,'SegEnds_NonXtal_BW#'!$A:$AR,33,FALSE)+AX11-50</f>
@@ -6284,13 +6284,13 @@
         <v>299</v>
       </c>
       <c r="AZ11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BA11" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BB11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BD11" t="str">
         <f>IF(COUNTIF('SegEnds_Xtal_Prot#'!B:B,'SegEnds_NonXtal_Prot#'!B11)&gt;0,IF(COUNTIF(BK11:BX11,TRUE)=14,TRUE,FALSE),"NoXtal")</f>
@@ -6383,7 +6383,7 @@
         <v>S6EXB4_ZYGB2__wt</v>
       </c>
       <c r="B12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C12" t="str">
         <f>VLOOKUP(B12,Seqs!A:B,2,FALSE)</f>
@@ -6434,13 +6434,13 @@
         <v>65</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S12">
         <f>VLOOKUP($B12,'SegEnds_NonXtal_BW#'!$A:$AR,13,FALSE)+T12-50</f>
@@ -6476,13 +6476,13 @@
         <v>148</v>
       </c>
       <c r="AB12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AC12" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AE12" s="1">
         <f>VLOOKUP($B12,'SegEnds_NonXtal_BW#'!$A:$AR,21,FALSE)+AF12-50</f>
@@ -6496,13 +6496,13 @@
         <v>188</v>
       </c>
       <c r="AH12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AI12" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AJ12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AK12">
         <f>VLOOKUP($B12,'SegEnds_NonXtal_BW#'!$A:$AR,25,FALSE)+AL12-50</f>
@@ -6516,13 +6516,13 @@
         <v>229</v>
       </c>
       <c r="AN12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AO12" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AP12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AQ12">
         <f>VLOOKUP($B12,'SegEnds_NonXtal_BW#'!$A:$AR,29,FALSE)+AR12-50</f>
@@ -6536,13 +6536,13 @@
         <v>261</v>
       </c>
       <c r="AT12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AU12" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AV12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AW12">
         <f>VLOOKUP($B12,'SegEnds_NonXtal_BW#'!$A:$AR,33,FALSE)+AX12-50</f>
@@ -6556,13 +6556,13 @@
         <v>299</v>
       </c>
       <c r="AZ12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BA12" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BB12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BD12" t="str">
         <f>IF(COUNTIF('SegEnds_Xtal_Prot#'!B:B,'SegEnds_NonXtal_Prot#'!B12)&gt;0,IF(COUNTIF(BK12:BX12,TRUE)=14,TRUE,FALSE),"NoXtal")</f>
@@ -6655,7 +6655,7 @@
         <v>C5DX97_ZYGRC__wt</v>
       </c>
       <c r="B13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C13" t="str">
         <f>VLOOKUP(B13,Seqs!A:B,2,FALSE)</f>
@@ -6706,13 +6706,13 @@
         <v>64</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S13">
         <f>VLOOKUP($B13,'SegEnds_NonXtal_BW#'!$A:$AR,13,FALSE)+T13-50</f>
@@ -6748,13 +6748,13 @@
         <v>147</v>
       </c>
       <c r="AB13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AC13" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AE13" s="1">
         <f>VLOOKUP($B13,'SegEnds_NonXtal_BW#'!$A:$AR,21,FALSE)+AF13-50</f>
@@ -6768,13 +6768,13 @@
         <v>187</v>
       </c>
       <c r="AH13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AI13" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AJ13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AK13">
         <f>VLOOKUP($B13,'SegEnds_NonXtal_BW#'!$A:$AR,25,FALSE)+AL13-50</f>
@@ -6788,13 +6788,13 @@
         <v>228</v>
       </c>
       <c r="AN13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AO13" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AP13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AQ13">
         <f>VLOOKUP($B13,'SegEnds_NonXtal_BW#'!$A:$AR,29,FALSE)+AR13-50</f>
@@ -6808,13 +6808,13 @@
         <v>260</v>
       </c>
       <c r="AT13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AU13" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AV13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AW13">
         <f>VLOOKUP($B13,'SegEnds_NonXtal_BW#'!$A:$AR,33,FALSE)+AX13-50</f>
@@ -6828,13 +6828,13 @@
         <v>298</v>
       </c>
       <c r="AZ13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BA13" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BB13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BD13" t="str">
         <f>IF(COUNTIF('SegEnds_Xtal_Prot#'!B:B,'SegEnds_NonXtal_Prot#'!B13)&gt;0,IF(COUNTIF(BK13:BX13,TRUE)=14,TRUE,FALSE),"NoXtal")</f>
@@ -6963,76 +6963,76 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L1" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="R1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="T1" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="U1" s="10" t="s">
         <v>61</v>
-      </c>
-      <c r="U1" s="10" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="str">
         <f>VLOOKUP(A2,Seqs!A:B,2,FALSE)</f>
         <v>ste2_yeast</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D2" t="str">
         <f>IF(ISERROR(MATCH(A2,'SegEnds_Xtal_Prot#'!B:B, 0)), "NoXtal", "Xtal")</f>
@@ -7041,14 +7041,14 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" t="str">
         <f>VLOOKUP(A3,Seqs!A:B,2,FALSE)</f>
         <v>ste2_yeast</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" t="str">
         <f>IF(ISERROR(MATCH(A3,'SegEnds_Xtal_Prot#'!B:B, 0)), "NoXtal", "Xtal")</f>
@@ -7057,14 +7057,14 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" t="str">
         <f>VLOOKUP(A4,Seqs!A:B,2,FALSE)</f>
         <v>ste2_yeast</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" t="str">
         <f>IF(ISERROR(MATCH(A4,'SegEnds_Xtal_Prot#'!B:B, 0)), "NoXtal", "Xtal")</f>
@@ -7073,14 +7073,14 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" t="str">
         <f>VLOOKUP(A5,Seqs!A:B,2,FALSE)</f>
         <v>ste2_yeast</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D5" t="str">
         <f>IF(ISERROR(MATCH(A5,'SegEnds_Xtal_Prot#'!B:B, 0)), "NoXtal", "Xtal")</f>
@@ -7089,14 +7089,14 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" t="str">
         <f>VLOOKUP(A6,Seqs!A:B,2,FALSE)</f>
         <v>ste2_yeast</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" t="str">
         <f>IF(ISERROR(MATCH(A6,'SegEnds_Xtal_Prot#'!B:B, 0)), "NoXtal", "Xtal")</f>
@@ -7105,14 +7105,14 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" t="str">
         <f>VLOOKUP(A7,Seqs!A:B,2,FALSE)</f>
         <v>ste2_yeast</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" t="str">
         <f>IF(ISERROR(MATCH(A7,'SegEnds_Xtal_Prot#'!B:B, 0)), "NoXtal", "Xtal")</f>
@@ -7121,14 +7121,14 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" t="str">
         <f>VLOOKUP(A8,Seqs!A:B,2,FALSE)</f>
         <v>ste2_yeast</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8" t="str">
         <f>IF(ISERROR(MATCH(A8,'SegEnds_Xtal_Prot#'!B:B, 0)), "NoXtal", "Xtal")</f>
@@ -7137,14 +7137,14 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" t="str">
         <f>VLOOKUP(A9,Seqs!A:B,2,FALSE)</f>
         <v>ste2_yeast</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D9" t="str">
         <f>IF(ISERROR(MATCH(A9,'SegEnds_Xtal_Prot#'!B:B, 0)), "NoXtal", "Xtal")</f>
@@ -7153,14 +7153,14 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B10" t="str">
         <f>VLOOKUP(A10,Seqs!A:B,2,FALSE)</f>
         <v>ste2_yeast</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" t="str">
         <f>IF(ISERROR(MATCH(A10,'SegEnds_Xtal_Prot#'!B:B, 0)), "NoXtal", "Xtal")</f>
@@ -7169,14 +7169,14 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B11" t="str">
         <f>VLOOKUP(A11,Seqs!A:B,2,FALSE)</f>
         <v>ste2_yeast</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D11" t="str">
         <f>IF(ISERROR(MATCH(A11,'SegEnds_Xtal_Prot#'!B:B, 0)), "NoXtal", "Xtal")</f>
@@ -7185,14 +7185,14 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B12" t="str">
         <f>VLOOKUP(A12,Seqs!A:B,2,FALSE)</f>
         <v>ste2_yeast</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D12" t="str">
         <f>IF(ISERROR(MATCH(A12,'SegEnds_Xtal_Prot#'!B:B, 0)), "NoXtal", "Xtal")</f>
@@ -7201,14 +7201,14 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B13" t="str">
         <f>VLOOKUP(A13,Seqs!A:B,2,FALSE)</f>
         <v>ste2_yeast</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" t="str">
         <f>IF(ISERROR(MATCH(A13,'SegEnds_Xtal_Prot#'!B:B, 0)), "NoXtal", "Xtal")</f>
@@ -7239,24 +7239,24 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="str">
         <f>IF(ISERROR(MATCH(A2,'SegEnds_Xtal_Prot#'!B:B, 0)), "NoXtal", "Xtal")</f>
@@ -7265,13 +7265,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
         <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
       </c>
       <c r="D3" t="str">
         <f>IF(ISERROR(MATCH(A3,'SegEnds_Xtal_Prot#'!B:B, 0)), "NoXtal", "Xtal")</f>
@@ -7280,13 +7280,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>34</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>35</v>
       </c>
       <c r="D4" t="str">
         <f>IF(ISERROR(MATCH(A4,'SegEnds_Xtal_Prot#'!B:B, 0)), "NoXtal", "Xtal")</f>
@@ -7295,13 +7295,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
         <v>36</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
       </c>
       <c r="D5" t="str">
         <f>IF(ISERROR(MATCH(A5,'SegEnds_Xtal_Prot#'!B:B, 0)), "NoXtal", "Xtal")</f>
@@ -7310,13 +7310,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
         <v>38</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
       </c>
       <c r="D6" t="str">
         <f>IF(ISERROR(MATCH(A6,'SegEnds_Xtal_Prot#'!B:B, 0)), "NoXtal", "Xtal")</f>
@@ -7325,13 +7325,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>40</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>41</v>
       </c>
       <c r="D7" t="str">
         <f>IF(ISERROR(MATCH(A7,'SegEnds_Xtal_Prot#'!B:B, 0)), "NoXtal", "Xtal")</f>
@@ -7340,13 +7340,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
         <v>42</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>43</v>
       </c>
       <c r="D8" t="str">
         <f>IF(ISERROR(MATCH(A8,'SegEnds_Xtal_Prot#'!B:B, 0)), "NoXtal", "Xtal")</f>
@@ -7355,13 +7355,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>84</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>85</v>
       </c>
       <c r="D9" t="str">
         <f>IF(ISERROR(MATCH(A9,'SegEnds_Xtal_Prot#'!B:B, 0)), "NoXtal", "Xtal")</f>
@@ -7370,13 +7370,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D10" t="str">
         <f>IF(ISERROR(MATCH(A10,'SegEnds_Xtal_Prot#'!B:B, 0)), "NoXtal", "Xtal")</f>
@@ -7385,13 +7385,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D11" t="str">
         <f>IF(ISERROR(MATCH(A11,'SegEnds_Xtal_Prot#'!B:B, 0)), "NoXtal", "Xtal")</f>
@@ -7400,13 +7400,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D12" t="str">
         <f>IF(ISERROR(MATCH(A12,'SegEnds_Xtal_Prot#'!B:B, 0)), "NoXtal", "Xtal")</f>
@@ -7415,13 +7415,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D13" t="str">
         <f>IF(ISERROR(MATCH(A13,'SegEnds_Xtal_Prot#'!B:B, 0)), "NoXtal", "Xtal")</f>

</xml_diff>